<commit_message>
A variety of changes
Including the height changes.
</commit_message>
<xml_diff>
--- a/data/network.xlsx
+++ b/data/network.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10210"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10410"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Rick/Sync/public_html/shiny_cv/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Rick/Documents/GitHub/shiny_cv/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A7D9E26-01F6-7145-B585-9433775673BE}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="10160" windowWidth="33600" windowHeight="9740" xr2:uid="{0757B4E7-21A4-3F45-9C41-5341E0219DA4}"/>
+    <workbookView xWindow="40" yWindow="1200" windowWidth="33600" windowHeight="18020" xr2:uid="{0757B4E7-21A4-3F45-9C41-5341E0219DA4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="39">
   <si>
     <t>node</t>
   </si>
@@ -41,18 +42,9 @@
     <t>MSc</t>
   </si>
   <si>
-    <t>Easter Bush</t>
-  </si>
-  <si>
     <t>BSc</t>
   </si>
   <si>
-    <t>Silvertown et al</t>
-  </si>
-  <si>
-    <t>Isogai et al</t>
-  </si>
-  <si>
     <t>group</t>
   </si>
   <si>
@@ -68,9 +60,6 @@
     <t>Easter Bush Research Consortium and Pfizer Bursary</t>
   </si>
   <si>
-    <t>Pfizer Prize</t>
-  </si>
-  <si>
     <t>6th Orthomyxovirus Travel Grant</t>
   </si>
   <si>
@@ -95,15 +84,9 @@
     <t>ACCM</t>
   </si>
   <si>
-    <t>Mechanisms of Disease</t>
-  </si>
-  <si>
     <t>teaching</t>
   </si>
   <si>
-    <t>BIOM</t>
-  </si>
-  <si>
     <t>OVC PhD Fellowship</t>
   </si>
   <si>
@@ -113,13 +96,52 @@
     <t>Queen Elizabeth II Scholarship</t>
   </si>
   <si>
-    <t>Wills et al</t>
-  </si>
-  <si>
-    <t>Fraser et al B</t>
-  </si>
-  <si>
-    <t>Fraser et al A</t>
+    <t>Wellcome Trust Essay</t>
+  </si>
+  <si>
+    <t>Pfizer Prize for Best Student</t>
+  </si>
+  <si>
+    <t>Meakins-Christie Lab, McGill</t>
+  </si>
+  <si>
+    <t>degree</t>
+  </si>
+  <si>
+    <t>Anatomic Pathology Rotation</t>
+  </si>
+  <si>
+    <t>Silvertown et al (2005)</t>
+  </si>
+  <si>
+    <t>Fraser et al (2018a)</t>
+  </si>
+  <si>
+    <t>Isogai et al (2007)</t>
+  </si>
+  <si>
+    <t>Wills et al (2018)</t>
+  </si>
+  <si>
+    <t>Fraser et al (2018b)</t>
+  </si>
+  <si>
+    <t>Bors et al (2017)</t>
+  </si>
+  <si>
+    <t>Digard Lab (Roslin Institute)</t>
+  </si>
+  <si>
+    <t>TA (Principles of Disease)</t>
+  </si>
+  <si>
+    <t>Lecturer (Mechanisms of Disease)</t>
+  </si>
+  <si>
+    <t>Guest lecturer (BIOM6800)</t>
+  </si>
+  <si>
+    <t>Summerlee Lab (University of Guelph)</t>
   </si>
 </sst>
 </file>
@@ -470,13 +492,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCFDBCB7-1BB4-6448-8BAC-2F088F8F1726}">
-  <dimension ref="B2:D23"/>
+  <dimension ref="B2:D34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col min="2" max="2" width="23.140625" customWidth="1"/>
+    <col min="3" max="3" width="65.5703125" customWidth="1"/>
+    <col min="4" max="4" width="20.28515625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="2" spans="2:4">
       <c r="B2" t="s">
@@ -486,7 +513,7 @@
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="2:4">
@@ -494,10 +521,10 @@
         <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D3" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="2:4">
@@ -505,10 +532,10 @@
         <v>2</v>
       </c>
       <c r="C4" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="D4" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="2:4">
@@ -516,10 +543,10 @@
         <v>2</v>
       </c>
       <c r="C5" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="D5" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="2:4">
@@ -527,43 +554,43 @@
         <v>3</v>
       </c>
       <c r="C6" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="D6" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="7" spans="2:4">
       <c r="B7" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C7" t="s">
-        <v>5</v>
+        <v>28</v>
       </c>
       <c r="D7" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
     </row>
     <row r="8" spans="2:4">
       <c r="B8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C8" t="s">
+        <v>30</v>
+      </c>
+      <c r="D8" t="s">
         <v>7</v>
-      </c>
-      <c r="D8" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="9" spans="2:4">
       <c r="B9" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C9" t="s">
+        <v>10</v>
+      </c>
+      <c r="D9" t="s">
         <v>8</v>
-      </c>
-      <c r="D9" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="10" spans="2:4">
@@ -571,10 +598,10 @@
         <v>4</v>
       </c>
       <c r="C10" t="s">
-        <v>13</v>
+        <v>24</v>
       </c>
       <c r="D10" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="11" spans="2:4">
@@ -582,21 +609,21 @@
         <v>4</v>
       </c>
       <c r="C11" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="D11" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="12" spans="2:4">
       <c r="B12" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C12" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="D12" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="13" spans="2:4">
@@ -607,18 +634,18 @@
         <v>16</v>
       </c>
       <c r="D13" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="14" spans="2:4">
       <c r="B14" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C14" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="D14" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="15" spans="2:4">
@@ -626,21 +653,21 @@
         <v>3</v>
       </c>
       <c r="C15" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D15" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="16" spans="2:4">
       <c r="B16" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C16" t="s">
-        <v>22</v>
+        <v>36</v>
       </c>
       <c r="D16" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
     </row>
     <row r="17" spans="2:4">
@@ -648,10 +675,10 @@
         <v>2</v>
       </c>
       <c r="C17" t="s">
-        <v>23</v>
+        <v>37</v>
       </c>
       <c r="D17" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
     </row>
     <row r="18" spans="2:4">
@@ -659,10 +686,10 @@
         <v>2</v>
       </c>
       <c r="C18" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="D18" t="s">
-        <v>24</v>
+        <v>8</v>
       </c>
     </row>
     <row r="19" spans="2:4">
@@ -670,10 +697,10 @@
         <v>2</v>
       </c>
       <c r="C19" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="D19" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="20" spans="2:4">
@@ -681,10 +708,10 @@
         <v>2</v>
       </c>
       <c r="C20" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="D20" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="21" spans="2:4">
@@ -692,10 +719,10 @@
         <v>2</v>
       </c>
       <c r="C21" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="D21" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
     </row>
     <row r="22" spans="2:4">
@@ -703,21 +730,142 @@
         <v>2</v>
       </c>
       <c r="C22" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="D22" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="23" spans="2:4">
       <c r="B23" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C23" t="s">
+        <v>23</v>
+      </c>
+      <c r="D23" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="24" spans="2:4">
+      <c r="B24" t="s">
+        <v>2</v>
+      </c>
+      <c r="C24" t="s">
+        <v>33</v>
+      </c>
+      <c r="D24" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="25" spans="2:4">
+      <c r="B25" t="s">
+        <v>5</v>
+      </c>
+      <c r="C25" t="s">
+        <v>25</v>
+      </c>
+      <c r="D25" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="26" spans="2:4">
+      <c r="B26" t="s">
+        <v>5</v>
+      </c>
+      <c r="C26" t="s">
+        <v>38</v>
+      </c>
+      <c r="D26" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="27" spans="2:4">
+      <c r="B27" t="s">
+        <v>4</v>
+      </c>
+      <c r="C27" t="s">
+        <v>34</v>
+      </c>
+      <c r="D27" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="28" spans="2:4">
+      <c r="B28" t="s">
+        <v>25</v>
+      </c>
+      <c r="C28" t="s">
         <v>30</v>
       </c>
-      <c r="D23" t="s">
-        <v>10</v>
+      <c r="D28" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="29" spans="2:4">
+      <c r="B29" t="s">
+        <v>5</v>
+      </c>
+      <c r="C29" t="s">
+        <v>3</v>
+      </c>
+      <c r="D29" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="30" spans="2:4">
+      <c r="B30" t="s">
+        <v>3</v>
+      </c>
+      <c r="C30" t="s">
+        <v>4</v>
+      </c>
+      <c r="D30" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="31" spans="2:4">
+      <c r="B31" t="s">
+        <v>4</v>
+      </c>
+      <c r="C31" t="s">
+        <v>2</v>
+      </c>
+      <c r="D31" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="32" spans="2:4">
+      <c r="B32" t="s">
+        <v>38</v>
+      </c>
+      <c r="C32" t="s">
+        <v>28</v>
+      </c>
+      <c r="D32" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="33" spans="2:4">
+      <c r="B33" t="s">
+        <v>2</v>
+      </c>
+      <c r="C33" t="s">
+        <v>27</v>
+      </c>
+      <c r="D33" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="34" spans="2:4">
+      <c r="B34" t="s">
+        <v>2</v>
+      </c>
+      <c r="C34" t="s">
+        <v>35</v>
+      </c>
+      <c r="D34" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>